<commit_message>
final project 2 commit
</commit_message>
<xml_diff>
--- a/scripts/projeto2/dados/legislativas.xlsx
+++ b/scripts/projeto2/dados/legislativas.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hpacheco/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Github\progii\scripts\projeto2\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE3FF18-30D5-5647-913D-A59D6E33D495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB32843-78C7-4FD4-93BA-8C017E0AE2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Quadro" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Quadro!$A$2:$AJ$359</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -1336,7 +1339,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1652,20 +1655,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AJ359"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="AJ5" sqref="AJ5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="36" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="36" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:36" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1709,7 +1713,7 @@
       <c r="AI1" s="11"/>
       <c r="AJ1" s="11"/>
     </row>
-    <row r="2" spans="1:36" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:36" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1819,7 +1823,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1929,7 +1933,7 @@
         <v>5563497</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -2039,7 +2043,7 @@
         <v>5178510</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2149,7 +2153,7 @@
         <v>2001871</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -2259,7 +2263,7 @@
         <v>127040</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -2369,7 +2373,7 @@
         <v>11262</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
@@ -2479,7 +2483,7 @@
         <v>9066</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -2589,7 +2593,7 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="10" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -2699,7 +2703,7 @@
         <v>8855</v>
       </c>
     </row>
-    <row r="11" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -2809,7 +2813,7 @@
         <v>4457</v>
       </c>
     </row>
-    <row r="12" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -2919,7 +2923,7 @@
         <v>6445</v>
       </c>
     </row>
-    <row r="13" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -3029,7 +3033,7 @@
         <v>24453</v>
       </c>
     </row>
-    <row r="14" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
@@ -3139,7 +3143,7 @@
         <v>6451</v>
       </c>
     </row>
-    <row r="15" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -3249,7 +3253,7 @@
         <v>47639</v>
       </c>
     </row>
-    <row r="16" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
@@ -3359,7 +3363,7 @@
         <v>4734</v>
       </c>
     </row>
-    <row r="17" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
@@ -3469,7 +3473,7 @@
         <v>238047</v>
       </c>
     </row>
-    <row r="18" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
@@ -3579,7 +3583,7 @@
         <v>10837</v>
       </c>
     </row>
-    <row r="19" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
@@ -3689,7 +3693,7 @@
         <v>70953</v>
       </c>
     </row>
-    <row r="20" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>13</v>
       </c>
@@ -3799,7 +3803,7 @@
         <v>106812</v>
       </c>
     </row>
-    <row r="21" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>13</v>
       </c>
@@ -3909,7 +3913,7 @@
         <v>19621</v>
       </c>
     </row>
-    <row r="22" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>13</v>
       </c>
@@ -4019,7 +4023,7 @@
         <v>3846</v>
       </c>
     </row>
-    <row r="23" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>13</v>
       </c>
@@ -4129,7 +4133,7 @@
         <v>25978</v>
       </c>
     </row>
-    <row r="24" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>11</v>
       </c>
@@ -4239,7 +4243,7 @@
         <v>250501</v>
       </c>
     </row>
-    <row r="25" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
@@ -4349,7 +4353,7 @@
         <v>9253</v>
       </c>
     </row>
-    <row r="26" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>13</v>
       </c>
@@ -4459,7 +4463,7 @@
         <v>28642</v>
       </c>
     </row>
-    <row r="27" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -4569,7 +4573,7 @@
         <v>96870</v>
       </c>
     </row>
-    <row r="28" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>13</v>
       </c>
@@ -4679,7 +4683,7 @@
         <v>3689</v>
       </c>
     </row>
-    <row r="29" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>13</v>
       </c>
@@ -4789,7 +4793,7 @@
         <v>12856</v>
       </c>
     </row>
-    <row r="30" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>13</v>
       </c>
@@ -4899,7 +4903,7 @@
         <v>6996</v>
       </c>
     </row>
-    <row r="31" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>13</v>
       </c>
@@ -5009,7 +5013,7 @@
         <v>78289</v>
       </c>
     </row>
-    <row r="32" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>13</v>
       </c>
@@ -5119,7 +5123,7 @@
         <v>13906</v>
       </c>
     </row>
-    <row r="33" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>11</v>
       </c>
@@ -5229,7 +5233,7 @@
         <v>956441</v>
       </c>
     </row>
-    <row r="34" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>13</v>
       </c>
@@ -5339,7 +5343,7 @@
         <v>12021</v>
       </c>
     </row>
-    <row r="35" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>13</v>
       </c>
@@ -5449,7 +5453,7 @@
         <v>18206</v>
       </c>
     </row>
-    <row r="36" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>13</v>
       </c>
@@ -5559,7 +5563,7 @@
         <v>88549</v>
       </c>
     </row>
-    <row r="37" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>13</v>
       </c>
@@ -5669,7 +5673,7 @@
         <v>77474</v>
       </c>
     </row>
-    <row r="38" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>13</v>
       </c>
@@ -5779,7 +5783,7 @@
         <v>94474</v>
       </c>
     </row>
-    <row r="39" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>13</v>
       </c>
@@ -5889,7 +5893,7 @@
         <v>35177</v>
       </c>
     </row>
-    <row r="40" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>13</v>
       </c>
@@ -5999,7 +6003,7 @@
         <v>47085</v>
       </c>
     </row>
-    <row r="41" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>13</v>
       </c>
@@ -6109,7 +6113,7 @@
         <v>132157</v>
       </c>
     </row>
-    <row r="42" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>13</v>
       </c>
@@ -6219,7 +6223,7 @@
         <v>33825</v>
       </c>
     </row>
-    <row r="43" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>13</v>
       </c>
@@ -6329,7 +6333,7 @@
         <v>74548</v>
       </c>
     </row>
-    <row r="44" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>13</v>
       </c>
@@ -6439,7 +6443,7 @@
         <v>39280</v>
       </c>
     </row>
-    <row r="45" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>13</v>
       </c>
@@ -6549,7 +6553,7 @@
         <v>11535</v>
       </c>
     </row>
-    <row r="46" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>13</v>
       </c>
@@ -6659,7 +6663,7 @@
         <v>21442</v>
       </c>
     </row>
-    <row r="47" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>13</v>
       </c>
@@ -6769,7 +6773,7 @@
         <v>12116</v>
       </c>
     </row>
-    <row r="48" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>13</v>
       </c>
@@ -6879,7 +6883,7 @@
         <v>50455</v>
       </c>
     </row>
-    <row r="49" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>13</v>
       </c>
@@ -6989,7 +6993,7 @@
         <v>43168</v>
       </c>
     </row>
-    <row r="50" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>13</v>
       </c>
@@ -7099,7 +7103,7 @@
         <v>164929</v>
       </c>
     </row>
-    <row r="51" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>11</v>
       </c>
@@ -7209,7 +7213,7 @@
         <v>46967</v>
       </c>
     </row>
-    <row r="52" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>13</v>
       </c>
@@ -7319,7 +7323,7 @@
         <v>3320</v>
       </c>
     </row>
-    <row r="53" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>13</v>
       </c>
@@ -7429,7 +7433,7 @@
         <v>19617</v>
       </c>
     </row>
-    <row r="54" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>13</v>
       </c>
@@ -7539,7 +7543,7 @@
         <v>5625</v>
       </c>
     </row>
-    <row r="55" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>13</v>
       </c>
@@ -7649,7 +7653,7 @@
         <v>3429</v>
       </c>
     </row>
-    <row r="56" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>13</v>
       </c>
@@ -7759,7 +7763,7 @@
         <v>8069</v>
       </c>
     </row>
-    <row r="57" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>13</v>
       </c>
@@ -7869,7 +7873,7 @@
         <v>6907</v>
       </c>
     </row>
-    <row r="58" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>11</v>
       </c>
@@ -7979,7 +7983,7 @@
         <v>223337</v>
       </c>
     </row>
-    <row r="59" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>13</v>
       </c>
@@ -8089,7 +8093,7 @@
         <v>28662</v>
       </c>
     </row>
-    <row r="60" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>13</v>
       </c>
@@ -8199,7 +8203,7 @@
         <v>8750</v>
       </c>
     </row>
-    <row r="61" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>13</v>
       </c>
@@ -8309,7 +8313,7 @@
         <v>8076</v>
       </c>
     </row>
-    <row r="62" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>13</v>
       </c>
@@ -8419,7 +8423,7 @@
         <v>9653</v>
       </c>
     </row>
-    <row r="63" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>13</v>
       </c>
@@ -8529,7 +8533,7 @@
         <v>8231</v>
       </c>
     </row>
-    <row r="64" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>13</v>
       </c>
@@ -8639,7 +8643,7 @@
         <v>31875</v>
       </c>
     </row>
-    <row r="65" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>13</v>
       </c>
@@ -8749,7 +8753,7 @@
         <v>26374</v>
       </c>
     </row>
-    <row r="66" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>13</v>
       </c>
@@ -8859,7 +8863,7 @@
         <v>26118</v>
       </c>
     </row>
-    <row r="67" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>13</v>
       </c>
@@ -8969,7 +8973,7 @@
         <v>30289</v>
       </c>
     </row>
-    <row r="68" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>13</v>
       </c>
@@ -9079,7 +9083,7 @@
         <v>39894</v>
       </c>
     </row>
-    <row r="69" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>13</v>
       </c>
@@ -9189,7 +9193,7 @@
         <v>5415</v>
       </c>
     </row>
-    <row r="70" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>11</v>
       </c>
@@ -9299,7 +9303,7 @@
         <v>102283</v>
       </c>
     </row>
-    <row r="71" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>13</v>
       </c>
@@ -9409,7 +9413,7 @@
         <v>5983</v>
       </c>
     </row>
-    <row r="72" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>13</v>
       </c>
@@ -9519,7 +9523,7 @@
         <v>2994</v>
       </c>
     </row>
-    <row r="73" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>13</v>
       </c>
@@ -9629,7 +9633,7 @@
         <v>3114</v>
       </c>
     </row>
-    <row r="74" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>13</v>
       </c>
@@ -9739,7 +9743,7 @@
         <v>1602</v>
       </c>
     </row>
-    <row r="75" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>13</v>
       </c>
@@ -9849,7 +9853,7 @@
         <v>13311</v>
       </c>
     </row>
-    <row r="76" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>13</v>
       </c>
@@ -9959,7 +9963,7 @@
         <v>1912</v>
       </c>
     </row>
-    <row r="77" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>13</v>
       </c>
@@ -10069,7 +10073,7 @@
         <v>5119</v>
       </c>
     </row>
-    <row r="78" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>13</v>
       </c>
@@ -10179,7 +10183,7 @@
         <v>2899</v>
       </c>
     </row>
-    <row r="79" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>13</v>
       </c>
@@ -10289,7 +10293,7 @@
         <v>1388</v>
       </c>
     </row>
-    <row r="80" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>13</v>
       </c>
@@ -10399,7 +10403,7 @@
         <v>7593</v>
       </c>
     </row>
-    <row r="81" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>13</v>
       </c>
@@ -10509,7 +10513,7 @@
         <v>3253</v>
       </c>
     </row>
-    <row r="82" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>13</v>
       </c>
@@ -10619,7 +10623,7 @@
         <v>3748</v>
       </c>
     </row>
-    <row r="83" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>13</v>
       </c>
@@ -10729,7 +10733,7 @@
         <v>3352</v>
       </c>
     </row>
-    <row r="84" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>13</v>
       </c>
@@ -10839,7 +10843,7 @@
         <v>3303</v>
       </c>
     </row>
-    <row r="85" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>13</v>
       </c>
@@ -10949,7 +10953,7 @@
         <v>2561</v>
       </c>
     </row>
-    <row r="86" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>13</v>
       </c>
@@ -11059,7 +11063,7 @@
         <v>3741</v>
       </c>
     </row>
-    <row r="87" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>13</v>
       </c>
@@ -11169,7 +11173,7 @@
         <v>3771</v>
       </c>
     </row>
-    <row r="88" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
         <v>13</v>
       </c>
@@ -11279,7 +11283,7 @@
         <v>3364</v>
       </c>
     </row>
-    <row r="89" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>13</v>
       </c>
@@ -11389,7 +11393,7 @@
         <v>29275</v>
       </c>
     </row>
-    <row r="90" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>11</v>
       </c>
@@ -11499,7 +11503,7 @@
         <v>57255</v>
       </c>
     </row>
-    <row r="91" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>13</v>
       </c>
@@ -11609,7 +11613,7 @@
         <v>2855</v>
       </c>
     </row>
-    <row r="92" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>13</v>
       </c>
@@ -11719,7 +11723,7 @@
         <v>16491</v>
       </c>
     </row>
-    <row r="93" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>13</v>
       </c>
@@ -11829,7 +11833,7 @@
         <v>7880</v>
       </c>
     </row>
-    <row r="94" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>13</v>
       </c>
@@ -11939,7 +11943,7 @@
         <v>3621</v>
       </c>
     </row>
-    <row r="95" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>13</v>
       </c>
@@ -12049,7 +12053,7 @@
         <v>11422</v>
       </c>
     </row>
-    <row r="96" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>13</v>
       </c>
@@ -12159,7 +12163,7 @@
         <v>4989</v>
       </c>
     </row>
-    <row r="97" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>13</v>
       </c>
@@ -12269,7 +12273,7 @@
         <v>3367</v>
       </c>
     </row>
-    <row r="98" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
         <v>13</v>
       </c>
@@ -12379,7 +12383,7 @@
         <v>2318</v>
       </c>
     </row>
-    <row r="99" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>13</v>
       </c>
@@ -12489,7 +12493,7 @@
         <v>4312</v>
       </c>
     </row>
-    <row r="100" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
         <v>9</v>
       </c>
@@ -12599,7 +12603,7 @@
         <v>862807</v>
       </c>
     </row>
-    <row r="101" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>11</v>
       </c>
@@ -12709,7 +12713,7 @@
         <v>183330</v>
       </c>
     </row>
-    <row r="102" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
         <v>13</v>
       </c>
@@ -12819,7 +12823,7 @@
         <v>23300</v>
       </c>
     </row>
-    <row r="103" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>13</v>
       </c>
@@ -12929,7 +12933,7 @@
         <v>12334</v>
       </c>
     </row>
-    <row r="104" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
         <v>13</v>
       </c>
@@ -13039,7 +13043,7 @@
         <v>14064</v>
       </c>
     </row>
-    <row r="105" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>13</v>
       </c>
@@ -13149,7 +13153,7 @@
         <v>40935</v>
       </c>
     </row>
-    <row r="106" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>13</v>
       </c>
@@ -13259,7 +13263,7 @@
         <v>12263</v>
       </c>
     </row>
-    <row r="107" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>13</v>
       </c>
@@ -13369,7 +13373,7 @@
         <v>18135</v>
       </c>
     </row>
-    <row r="108" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
         <v>13</v>
       </c>
@@ -13479,7 +13483,7 @@
         <v>4277</v>
       </c>
     </row>
-    <row r="109" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>13</v>
       </c>
@@ -13589,7 +13593,7 @@
         <v>11213</v>
       </c>
     </row>
-    <row r="110" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
         <v>13</v>
       </c>
@@ -13699,7 +13703,7 @@
         <v>29038</v>
       </c>
     </row>
-    <row r="111" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>13</v>
       </c>
@@ -13809,7 +13813,7 @@
         <v>6522</v>
       </c>
     </row>
-    <row r="112" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
         <v>13</v>
       </c>
@@ -13919,7 +13923,7 @@
         <v>11249</v>
       </c>
     </row>
-    <row r="113" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>11</v>
       </c>
@@ -14029,7 +14033,7 @@
         <v>229412</v>
       </c>
     </row>
-    <row r="114" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
         <v>13</v>
       </c>
@@ -14139,7 +14143,7 @@
         <v>5606</v>
       </c>
     </row>
-    <row r="115" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>13</v>
       </c>
@@ -14249,7 +14253,7 @@
         <v>17833</v>
       </c>
     </row>
-    <row r="116" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
         <v>13</v>
       </c>
@@ -14359,7 +14363,7 @@
         <v>76837</v>
       </c>
     </row>
-    <row r="117" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>13</v>
       </c>
@@ -14469,7 +14473,7 @@
         <v>8834</v>
       </c>
     </row>
-    <row r="118" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
         <v>13</v>
       </c>
@@ -14579,7 +14583,7 @@
         <v>30361</v>
       </c>
     </row>
-    <row r="119" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>13</v>
       </c>
@@ -14689,7 +14693,7 @@
         <v>2098</v>
       </c>
     </row>
-    <row r="120" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
         <v>13</v>
       </c>
@@ -14799,7 +14803,7 @@
         <v>8551</v>
       </c>
     </row>
-    <row r="121" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>13</v>
       </c>
@@ -14909,7 +14913,7 @@
         <v>9849</v>
       </c>
     </row>
-    <row r="122" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
         <v>13</v>
       </c>
@@ -15019,7 +15023,7 @@
         <v>6354</v>
       </c>
     </row>
-    <row r="123" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>13</v>
       </c>
@@ -15129,7 +15133,7 @@
         <v>6267</v>
       </c>
     </row>
-    <row r="124" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="s">
         <v>13</v>
       </c>
@@ -15239,7 +15243,7 @@
         <v>12494</v>
       </c>
     </row>
-    <row r="125" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>13</v>
       </c>
@@ -15349,7 +15353,7 @@
         <v>4441</v>
       </c>
     </row>
-    <row r="126" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A126" s="4" t="s">
         <v>13</v>
       </c>
@@ -15459,7 +15463,7 @@
         <v>10250</v>
       </c>
     </row>
-    <row r="127" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>13</v>
       </c>
@@ -15569,7 +15573,7 @@
         <v>1968</v>
       </c>
     </row>
-    <row r="128" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A128" s="4" t="s">
         <v>13</v>
       </c>
@@ -15679,7 +15683,7 @@
         <v>7263</v>
       </c>
     </row>
-    <row r="129" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>13</v>
       </c>
@@ -15789,7 +15793,7 @@
         <v>2653</v>
       </c>
     </row>
-    <row r="130" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A130" s="4" t="s">
         <v>13</v>
       </c>
@@ -15899,7 +15903,7 @@
         <v>9054</v>
       </c>
     </row>
-    <row r="131" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>13</v>
       </c>
@@ -16009,7 +16013,7 @@
         <v>5596</v>
       </c>
     </row>
-    <row r="132" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A132" s="4" t="s">
         <v>13</v>
       </c>
@@ -16119,7 +16123,7 @@
         <v>3103</v>
       </c>
     </row>
-    <row r="133" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>11</v>
       </c>
@@ -16229,7 +16233,7 @@
         <v>150197</v>
       </c>
     </row>
-    <row r="134" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
         <v>13</v>
       </c>
@@ -16339,7 +16343,7 @@
         <v>3355</v>
       </c>
     </row>
-    <row r="135" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>13</v>
       </c>
@@ -16449,7 +16453,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="136" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A136" s="4" t="s">
         <v>13</v>
       </c>
@@ -16559,7 +16563,7 @@
         <v>8656</v>
       </c>
     </row>
-    <row r="137" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>13</v>
       </c>
@@ -16669,7 +16673,7 @@
         <v>1545</v>
       </c>
     </row>
-    <row r="138" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
         <v>13</v>
       </c>
@@ -16779,7 +16783,7 @@
         <v>2957</v>
       </c>
     </row>
-    <row r="139" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>13</v>
       </c>
@@ -16889,7 +16893,7 @@
         <v>69066</v>
       </c>
     </row>
-    <row r="140" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A140" s="4" t="s">
         <v>13</v>
       </c>
@@ -16999,7 +17003,7 @@
         <v>19036</v>
       </c>
     </row>
-    <row r="141" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>13</v>
       </c>
@@ -17109,7 +17113,7 @@
         <v>1760</v>
       </c>
     </row>
-    <row r="142" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A142" s="4" t="s">
         <v>13</v>
       </c>
@@ -17219,7 +17223,7 @@
         <v>24856</v>
       </c>
     </row>
-    <row r="143" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>13</v>
       </c>
@@ -17329,7 +17333,7 @@
         <v>12466</v>
       </c>
     </row>
-    <row r="144" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
         <v>11</v>
       </c>
@@ -17439,7 +17443,7 @@
         <v>133503</v>
       </c>
     </row>
-    <row r="145" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>13</v>
       </c>
@@ -17549,7 +17553,7 @@
         <v>2915</v>
       </c>
     </row>
-    <row r="146" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A146" s="4" t="s">
         <v>13</v>
       </c>
@@ -17659,7 +17663,7 @@
         <v>4595</v>
       </c>
     </row>
-    <row r="147" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>13</v>
       </c>
@@ -17769,7 +17773,7 @@
         <v>6865</v>
       </c>
     </row>
-    <row r="148" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A148" s="4" t="s">
         <v>13</v>
       </c>
@@ -17879,7 +17883,7 @@
         <v>9112</v>
       </c>
     </row>
-    <row r="149" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>13</v>
       </c>
@@ -17989,7 +17993,7 @@
         <v>6582</v>
       </c>
     </row>
-    <row r="150" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A150" s="4" t="s">
         <v>13</v>
       </c>
@@ -18099,7 +18103,7 @@
         <v>5183</v>
       </c>
     </row>
-    <row r="151" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>13</v>
       </c>
@@ -18209,7 +18213,7 @@
         <v>4078</v>
       </c>
     </row>
-    <row r="152" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
         <v>13</v>
       </c>
@@ -18319,7 +18323,7 @@
         <v>5429</v>
       </c>
     </row>
-    <row r="153" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
         <v>13</v>
       </c>
@@ -18429,7 +18433,7 @@
         <v>8304</v>
       </c>
     </row>
-    <row r="154" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
         <v>13</v>
       </c>
@@ -18539,7 +18543,7 @@
         <v>5874</v>
       </c>
     </row>
-    <row r="155" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>13</v>
       </c>
@@ -18649,7 +18653,7 @@
         <v>14205</v>
       </c>
     </row>
-    <row r="156" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A156" s="4" t="s">
         <v>13</v>
       </c>
@@ -18759,7 +18763,7 @@
         <v>2595</v>
       </c>
     </row>
-    <row r="157" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>13</v>
       </c>
@@ -18869,7 +18873,7 @@
         <v>52509</v>
       </c>
     </row>
-    <row r="158" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A158" s="4" t="s">
         <v>13</v>
       </c>
@@ -18979,7 +18983,7 @@
         <v>5257</v>
       </c>
     </row>
-    <row r="159" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>11</v>
       </c>
@@ -19089,7 +19093,7 @@
         <v>52800</v>
       </c>
     </row>
-    <row r="160" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A160" s="4" t="s">
         <v>13</v>
       </c>
@@ -19199,7 +19203,7 @@
         <v>27532</v>
       </c>
     </row>
-    <row r="161" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>13</v>
       </c>
@@ -19309,7 +19313,7 @@
         <v>4284</v>
       </c>
     </row>
-    <row r="162" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A162" s="4" t="s">
         <v>13</v>
       </c>
@@ -19419,7 +19423,7 @@
         <v>2781</v>
       </c>
     </row>
-    <row r="163" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>13</v>
       </c>
@@ -19529,7 +19533,7 @@
         <v>2410</v>
       </c>
     </row>
-    <row r="164" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A164" s="4" t="s">
         <v>13</v>
       </c>
@@ -19639,7 +19643,7 @@
         <v>4126</v>
       </c>
     </row>
-    <row r="165" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
         <v>13</v>
       </c>
@@ -19749,7 +19753,7 @@
         <v>8168</v>
       </c>
     </row>
-    <row r="166" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A166" s="4" t="s">
         <v>13</v>
       </c>
@@ -19859,7 +19863,7 @@
         <v>1865</v>
       </c>
     </row>
-    <row r="167" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
         <v>13</v>
       </c>
@@ -19969,7 +19973,7 @@
         <v>1634</v>
       </c>
     </row>
-    <row r="168" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A168" s="4" t="s">
         <v>11</v>
       </c>
@@ -20079,7 +20083,7 @@
         <v>113565</v>
       </c>
     </row>
-    <row r="169" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
         <v>13</v>
       </c>
@@ -20189,7 +20193,7 @@
         <v>3295</v>
       </c>
     </row>
-    <row r="170" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A170" s="4" t="s">
         <v>13</v>
       </c>
@@ -20299,7 +20303,7 @@
         <v>3118</v>
       </c>
     </row>
-    <row r="171" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
         <v>13</v>
       </c>
@@ -20409,7 +20413,7 @@
         <v>3559</v>
       </c>
     </row>
-    <row r="172" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A172" s="4" t="s">
         <v>13</v>
       </c>
@@ -20519,7 +20523,7 @@
         <v>25829</v>
       </c>
     </row>
-    <row r="173" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
         <v>13</v>
       </c>
@@ -20629,7 +20633,7 @@
         <v>2760</v>
       </c>
     </row>
-    <row r="174" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A174" s="4" t="s">
         <v>13</v>
       </c>
@@ -20739,7 +20743,7 @@
         <v>2501</v>
       </c>
     </row>
-    <row r="175" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
         <v>13</v>
       </c>
@@ -20849,7 +20853,7 @@
         <v>13996</v>
       </c>
     </row>
-    <row r="176" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A176" s="4" t="s">
         <v>13</v>
       </c>
@@ -20959,7 +20963,7 @@
         <v>6223</v>
       </c>
     </row>
-    <row r="177" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
         <v>13</v>
       </c>
@@ -21069,7 +21073,7 @@
         <v>21784</v>
       </c>
     </row>
-    <row r="178" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A178" s="4" t="s">
         <v>13</v>
       </c>
@@ -21179,7 +21183,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="179" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
         <v>13</v>
       </c>
@@ -21289,7 +21293,7 @@
         <v>2458</v>
       </c>
     </row>
-    <row r="180" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A180" s="4" t="s">
         <v>13</v>
       </c>
@@ -21399,7 +21403,7 @@
         <v>4391</v>
       </c>
     </row>
-    <row r="181" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
         <v>13</v>
       </c>
@@ -21509,7 +21513,7 @@
         <v>5673</v>
       </c>
     </row>
-    <row r="182" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A182" s="4" t="s">
         <v>13</v>
       </c>
@@ -21619,7 +21623,7 @@
         <v>11748</v>
       </c>
     </row>
-    <row r="183" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
         <v>13</v>
       </c>
@@ -21729,7 +21733,7 @@
         <v>4652</v>
       </c>
     </row>
-    <row r="184" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" s="4" t="s">
         <v>9</v>
       </c>
@@ -21839,7 +21843,7 @@
         <v>412104</v>
       </c>
     </row>
-    <row r="185" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
         <v>11</v>
       </c>
@@ -21949,7 +21953,7 @@
         <v>183810</v>
       </c>
     </row>
-    <row r="186" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A186" s="4" t="s">
         <v>13</v>
       </c>
@@ -22059,7 +22063,7 @@
         <v>29043</v>
       </c>
     </row>
-    <row r="187" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
         <v>13</v>
       </c>
@@ -22169,7 +22173,7 @@
         <v>21820</v>
       </c>
     </row>
-    <row r="188" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A188" s="4" t="s">
         <v>13</v>
       </c>
@@ -22279,7 +22283,7 @@
         <v>7657</v>
       </c>
     </row>
-    <row r="189" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A189" s="2" t="s">
         <v>13</v>
       </c>
@@ -22389,7 +22393,7 @@
         <v>6389</v>
       </c>
     </row>
-    <row r="190" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A190" s="4" t="s">
         <v>13</v>
       </c>
@@ -22499,7 +22503,7 @@
         <v>6792</v>
       </c>
     </row>
-    <row r="191" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A191" s="2" t="s">
         <v>13</v>
       </c>
@@ -22609,7 +22613,7 @@
         <v>24804</v>
       </c>
     </row>
-    <row r="192" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="192" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A192" s="4" t="s">
         <v>13</v>
       </c>
@@ -22719,7 +22723,7 @@
         <v>13603</v>
       </c>
     </row>
-    <row r="193" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
         <v>13</v>
       </c>
@@ -22829,7 +22833,7 @@
         <v>6847</v>
       </c>
     </row>
-    <row r="194" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A194" s="4" t="s">
         <v>13</v>
       </c>
@@ -22939,7 +22943,7 @@
         <v>6071</v>
       </c>
     </row>
-    <row r="195" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
         <v>13</v>
       </c>
@@ -23049,7 +23053,7 @@
         <v>12430</v>
       </c>
     </row>
-    <row r="196" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A196" s="4" t="s">
         <v>13</v>
       </c>
@@ -23159,7 +23163,7 @@
         <v>5381</v>
       </c>
     </row>
-    <row r="197" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A197" s="2" t="s">
         <v>13</v>
       </c>
@@ -23269,7 +23273,7 @@
         <v>42973</v>
       </c>
     </row>
-    <row r="198" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A198" s="4" t="s">
         <v>11</v>
       </c>
@@ -23379,7 +23383,7 @@
         <v>112563</v>
       </c>
     </row>
-    <row r="199" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A199" s="2" t="s">
         <v>13</v>
       </c>
@@ -23489,7 +23493,7 @@
         <v>18319</v>
       </c>
     </row>
-    <row r="200" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="200" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A200" s="4" t="s">
         <v>13</v>
       </c>
@@ -23599,7 +23603,7 @@
         <v>6544</v>
       </c>
     </row>
-    <row r="201" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="201" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A201" s="2" t="s">
         <v>13</v>
       </c>
@@ -23709,7 +23713,7 @@
         <v>2112</v>
       </c>
     </row>
-    <row r="202" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="202" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A202" s="4" t="s">
         <v>13</v>
       </c>
@@ -23819,7 +23823,7 @@
         <v>10162</v>
       </c>
     </row>
-    <row r="203" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A203" s="2" t="s">
         <v>13</v>
       </c>
@@ -23929,7 +23933,7 @@
         <v>4334</v>
       </c>
     </row>
-    <row r="204" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="204" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A204" s="4" t="s">
         <v>13</v>
       </c>
@@ -24039,7 +24043,7 @@
         <v>3858</v>
       </c>
     </row>
-    <row r="205" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="205" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A205" s="2" t="s">
         <v>13</v>
       </c>
@@ -24149,7 +24153,7 @@
         <v>23312</v>
       </c>
     </row>
-    <row r="206" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="206" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A206" s="4" t="s">
         <v>13</v>
       </c>
@@ -24259,7 +24263,7 @@
         <v>2164</v>
       </c>
     </row>
-    <row r="207" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A207" s="2" t="s">
         <v>13</v>
       </c>
@@ -24369,7 +24373,7 @@
         <v>19337</v>
       </c>
     </row>
-    <row r="208" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A208" s="4" t="s">
         <v>13</v>
       </c>
@@ -24479,7 +24483,7 @@
         <v>18644</v>
       </c>
     </row>
-    <row r="209" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A209" s="2" t="s">
         <v>13</v>
       </c>
@@ -24589,7 +24593,7 @@
         <v>3777</v>
       </c>
     </row>
-    <row r="210" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A210" s="4" t="s">
         <v>11</v>
       </c>
@@ -24699,7 +24703,7 @@
         <v>115731</v>
       </c>
     </row>
-    <row r="211" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="211" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A211" s="2" t="s">
         <v>13</v>
       </c>
@@ -24809,7 +24813,7 @@
         <v>10043</v>
       </c>
     </row>
-    <row r="212" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="212" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A212" s="4" t="s">
         <v>13</v>
       </c>
@@ -24919,7 +24923,7 @@
         <v>3648</v>
       </c>
     </row>
-    <row r="213" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A213" s="2" t="s">
         <v>13</v>
       </c>
@@ -25029,7 +25033,7 @@
         <v>10102</v>
       </c>
     </row>
-    <row r="214" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A214" s="4" t="s">
         <v>13</v>
       </c>
@@ -25139,7 +25143,7 @@
         <v>13402</v>
       </c>
     </row>
-    <row r="215" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A215" s="2" t="s">
         <v>13</v>
       </c>
@@ -25249,7 +25253,7 @@
         <v>11861</v>
       </c>
     </row>
-    <row r="216" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A216" s="4" t="s">
         <v>13</v>
       </c>
@@ -25359,7 +25363,7 @@
         <v>4397</v>
       </c>
     </row>
-    <row r="217" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="217" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A217" s="2" t="s">
         <v>13</v>
       </c>
@@ -25469,7 +25473,7 @@
         <v>8906</v>
       </c>
     </row>
-    <row r="218" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="218" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A218" s="4" t="s">
         <v>13</v>
       </c>
@@ -25579,7 +25583,7 @@
         <v>2793</v>
       </c>
     </row>
-    <row r="219" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="219" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A219" s="2" t="s">
         <v>13</v>
       </c>
@@ -25689,7 +25693,7 @@
         <v>10286</v>
       </c>
     </row>
-    <row r="220" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="220" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A220" s="4" t="s">
         <v>13</v>
       </c>
@@ -25799,7 +25803,7 @@
         <v>9737</v>
       </c>
     </row>
-    <row r="221" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="221" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A221" s="2" t="s">
         <v>13</v>
       </c>
@@ -25909,7 +25913,7 @@
         <v>30556</v>
       </c>
     </row>
-    <row r="222" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="222" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" s="4" t="s">
         <v>9</v>
       </c>
@@ -26019,7 +26023,7 @@
         <v>1073546</v>
       </c>
     </row>
-    <row r="223" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="223" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A223" s="2" t="s">
         <v>11</v>
       </c>
@@ -26129,7 +26133,7 @@
         <v>1073546</v>
       </c>
     </row>
-    <row r="224" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="224" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A224" s="4" t="s">
         <v>13</v>
       </c>
@@ -26239,7 +26243,7 @@
         <v>83342</v>
       </c>
     </row>
-    <row r="225" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="225" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A225" s="2" t="s">
         <v>13</v>
       </c>
@@ -26349,7 +26353,7 @@
         <v>109126</v>
       </c>
     </row>
-    <row r="226" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="226" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A226" s="4" t="s">
         <v>13</v>
       </c>
@@ -26459,7 +26463,7 @@
         <v>303504</v>
       </c>
     </row>
-    <row r="227" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="227" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A227" s="2" t="s">
         <v>13</v>
       </c>
@@ -26569,7 +26573,7 @@
         <v>104238</v>
       </c>
     </row>
-    <row r="228" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="228" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A228" s="4" t="s">
         <v>13</v>
       </c>
@@ -26679,7 +26683,7 @@
         <v>44125</v>
       </c>
     </row>
-    <row r="229" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="229" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A229" s="2" t="s">
         <v>13</v>
       </c>
@@ -26789,7 +26793,7 @@
         <v>75924</v>
       </c>
     </row>
-    <row r="230" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="230" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A230" s="4" t="s">
         <v>13</v>
       </c>
@@ -26899,7 +26903,7 @@
         <v>97643</v>
       </c>
     </row>
-    <row r="231" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="231" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A231" s="2" t="s">
         <v>13</v>
       </c>
@@ -27009,7 +27013,7 @@
         <v>184556</v>
       </c>
     </row>
-    <row r="232" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="232" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A232" s="4" t="s">
         <v>13</v>
       </c>
@@ -27119,7 +27123,7 @@
         <v>71088</v>
       </c>
     </row>
-    <row r="233" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="233" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" s="2" t="s">
         <v>9</v>
       </c>
@@ -27229,7 +27233,7 @@
         <v>400941</v>
       </c>
     </row>
-    <row r="234" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="234" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A234" s="4" t="s">
         <v>11</v>
       </c>
@@ -27339,7 +27343,7 @@
         <v>400941</v>
       </c>
     </row>
-    <row r="235" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="235" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A235" s="2" t="s">
         <v>13</v>
       </c>
@@ -27449,7 +27453,7 @@
         <v>10136</v>
       </c>
     </row>
-    <row r="236" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="236" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A236" s="4" t="s">
         <v>13</v>
       </c>
@@ -27559,7 +27563,7 @@
         <v>89880</v>
       </c>
     </row>
-    <row r="237" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="237" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A237" s="2" t="s">
         <v>13</v>
       </c>
@@ -27669,7 +27673,7 @@
         <v>41198</v>
       </c>
     </row>
-    <row r="238" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="238" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A238" s="4" t="s">
         <v>13</v>
       </c>
@@ -27779,7 +27783,7 @@
         <v>31936</v>
       </c>
     </row>
-    <row r="239" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="239" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A239" s="2" t="s">
         <v>13</v>
       </c>
@@ -27889,7 +27893,7 @@
         <v>24704</v>
       </c>
     </row>
-    <row r="240" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="240" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A240" s="4" t="s">
         <v>13</v>
       </c>
@@ -27999,7 +28003,7 @@
         <v>32599</v>
       </c>
     </row>
-    <row r="241" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="241" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A241" s="2" t="s">
         <v>13</v>
       </c>
@@ -28109,7 +28113,7 @@
         <v>84702</v>
       </c>
     </row>
-    <row r="242" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="242" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A242" s="4" t="s">
         <v>13</v>
       </c>
@@ -28219,7 +28223,7 @@
         <v>26220</v>
       </c>
     </row>
-    <row r="243" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="243" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A243" s="2" t="s">
         <v>13</v>
       </c>
@@ -28329,7 +28333,7 @@
         <v>59566</v>
       </c>
     </row>
-    <row r="244" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="244" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" s="4" t="s">
         <v>9</v>
       </c>
@@ -28439,7 +28443,7 @@
         <v>232274</v>
       </c>
     </row>
-    <row r="245" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="245" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A245" s="2" t="s">
         <v>11</v>
       </c>
@@ -28549,7 +28553,7 @@
         <v>43410</v>
       </c>
     </row>
-    <row r="246" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="246" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A246" s="4" t="s">
         <v>13</v>
       </c>
@@ -28659,7 +28663,7 @@
         <v>5828</v>
       </c>
     </row>
-    <row r="247" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="247" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A247" s="2" t="s">
         <v>13</v>
       </c>
@@ -28769,7 +28773,7 @@
         <v>6625</v>
       </c>
     </row>
-    <row r="248" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="248" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A248" s="4" t="s">
         <v>13</v>
       </c>
@@ -28879,7 +28883,7 @@
         <v>11134</v>
       </c>
     </row>
-    <row r="249" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="249" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A249" s="2" t="s">
         <v>13</v>
       </c>
@@ -28989,7 +28993,7 @@
         <v>13769</v>
       </c>
     </row>
-    <row r="250" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="250" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A250" s="4" t="s">
         <v>13</v>
       </c>
@@ -29099,7 +29103,7 @@
         <v>6054</v>
       </c>
     </row>
-    <row r="251" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="251" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A251" s="2" t="s">
         <v>11</v>
       </c>
@@ -29209,7 +29213,7 @@
         <v>56396</v>
       </c>
     </row>
-    <row r="252" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="252" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A252" s="4" t="s">
         <v>13</v>
       </c>
@@ -29319,7 +29323,7 @@
         <v>4685</v>
       </c>
     </row>
-    <row r="253" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="253" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A253" s="2" t="s">
         <v>13</v>
       </c>
@@ -29429,7 +29433,7 @@
         <v>3424</v>
       </c>
     </row>
-    <row r="254" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="254" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A254" s="4" t="s">
         <v>13</v>
       </c>
@@ -29539,7 +29543,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="255" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="255" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A255" s="2" t="s">
         <v>13</v>
       </c>
@@ -29649,7 +29653,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="256" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="256" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A256" s="4" t="s">
         <v>13</v>
       </c>
@@ -29759,7 +29763,7 @@
         <v>15954</v>
       </c>
     </row>
-    <row r="257" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="257" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A257" s="2" t="s">
         <v>13</v>
       </c>
@@ -29869,7 +29873,7 @@
         <v>3499</v>
       </c>
     </row>
-    <row r="258" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="258" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A258" s="4" t="s">
         <v>13</v>
       </c>
@@ -29979,7 +29983,7 @@
         <v>2172</v>
       </c>
     </row>
-    <row r="259" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="259" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A259" s="2" t="s">
         <v>13</v>
       </c>
@@ -30089,7 +30093,7 @@
         <v>3437</v>
       </c>
     </row>
-    <row r="260" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="260" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A260" s="4" t="s">
         <v>13</v>
       </c>
@@ -30199,7 +30203,7 @@
         <v>3386</v>
       </c>
     </row>
-    <row r="261" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="261" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A261" s="2" t="s">
         <v>13</v>
       </c>
@@ -30309,7 +30313,7 @@
         <v>5921</v>
       </c>
     </row>
-    <row r="262" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="262" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A262" s="4" t="s">
         <v>13</v>
       </c>
@@ -30419,7 +30423,7 @@
         <v>2483</v>
       </c>
     </row>
-    <row r="263" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="263" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A263" s="2" t="s">
         <v>13</v>
       </c>
@@ -30529,7 +30533,7 @@
         <v>6999</v>
       </c>
     </row>
-    <row r="264" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="264" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A264" s="4" t="s">
         <v>13</v>
       </c>
@@ -30639,7 +30643,7 @@
         <v>2613</v>
       </c>
     </row>
-    <row r="265" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="265" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A265" s="2" t="s">
         <v>11</v>
       </c>
@@ -30749,7 +30753,7 @@
         <v>53528</v>
       </c>
     </row>
-    <row r="266" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="266" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A266" s="4" t="s">
         <v>13</v>
       </c>
@@ -30859,7 +30863,7 @@
         <v>1628</v>
       </c>
     </row>
-    <row r="267" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="267" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A267" s="2" t="s">
         <v>13</v>
       </c>
@@ -30969,7 +30973,7 @@
         <v>1468</v>
       </c>
     </row>
-    <row r="268" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="268" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A268" s="4" t="s">
         <v>13</v>
       </c>
@@ -31079,7 +31083,7 @@
         <v>2182</v>
       </c>
     </row>
-    <row r="269" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="269" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A269" s="2" t="s">
         <v>13</v>
       </c>
@@ -31189,7 +31193,7 @@
         <v>3802</v>
       </c>
     </row>
-    <row r="270" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="270" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A270" s="4" t="s">
         <v>13</v>
       </c>
@@ -31299,7 +31303,7 @@
         <v>1587</v>
       </c>
     </row>
-    <row r="271" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="271" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A271" s="2" t="s">
         <v>13</v>
       </c>
@@ -31409,7 +31413,7 @@
         <v>1906</v>
       </c>
     </row>
-    <row r="272" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="272" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A272" s="4" t="s">
         <v>13</v>
       </c>
@@ -31519,7 +31523,7 @@
         <v>9449</v>
       </c>
     </row>
-    <row r="273" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="273" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A273" s="2" t="s">
         <v>13</v>
       </c>
@@ -31629,7 +31633,7 @@
         <v>1564</v>
       </c>
     </row>
-    <row r="274" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="274" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A274" s="4" t="s">
         <v>13</v>
       </c>
@@ -31739,7 +31743,7 @@
         <v>1954</v>
       </c>
     </row>
-    <row r="275" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="275" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A275" s="2" t="s">
         <v>13</v>
       </c>
@@ -31849,7 +31853,7 @@
         <v>1586</v>
       </c>
     </row>
-    <row r="276" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="276" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A276" s="4" t="s">
         <v>13</v>
       </c>
@@ -31959,7 +31963,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="277" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="277" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A277" s="2" t="s">
         <v>13</v>
       </c>
@@ -32069,7 +32073,7 @@
         <v>3162</v>
       </c>
     </row>
-    <row r="278" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="278" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A278" s="4" t="s">
         <v>13</v>
       </c>
@@ -32179,7 +32183,7 @@
         <v>7471</v>
       </c>
     </row>
-    <row r="279" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="279" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A279" s="2" t="s">
         <v>13</v>
       </c>
@@ -32289,7 +32293,7 @@
         <v>12012</v>
       </c>
     </row>
-    <row r="280" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="280" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A280" s="4" t="s">
         <v>13</v>
       </c>
@@ -32399,7 +32403,7 @@
         <v>2335</v>
       </c>
     </row>
-    <row r="281" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="281" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A281" s="2" t="s">
         <v>11</v>
       </c>
@@ -32509,7 +32513,7 @@
         <v>78940</v>
       </c>
     </row>
-    <row r="282" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="282" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A282" s="4" t="s">
         <v>13</v>
       </c>
@@ -32619,7 +32623,7 @@
         <v>2668</v>
       </c>
     </row>
-    <row r="283" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="283" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A283" s="2" t="s">
         <v>13</v>
       </c>
@@ -32729,7 +32733,7 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="284" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="284" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A284" s="4" t="s">
         <v>13</v>
       </c>
@@ -32839,7 +32843,7 @@
         <v>3467</v>
       </c>
     </row>
-    <row r="285" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="285" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A285" s="2" t="s">
         <v>13</v>
       </c>
@@ -32949,7 +32953,7 @@
         <v>6412</v>
       </c>
     </row>
-    <row r="286" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="286" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A286" s="4" t="s">
         <v>13</v>
       </c>
@@ -33059,7 +33063,7 @@
         <v>27832</v>
       </c>
     </row>
-    <row r="287" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="287" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A287" s="2" t="s">
         <v>13</v>
       </c>
@@ -33169,7 +33173,7 @@
         <v>8534</v>
       </c>
     </row>
-    <row r="288" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="288" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A288" s="4" t="s">
         <v>13</v>
       </c>
@@ -33279,7 +33283,7 @@
         <v>2316</v>
       </c>
     </row>
-    <row r="289" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="289" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A289" s="2" t="s">
         <v>13</v>
       </c>
@@ -33389,7 +33393,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="290" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="290" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A290" s="4" t="s">
         <v>13</v>
       </c>
@@ -33499,7 +33503,7 @@
         <v>2959</v>
       </c>
     </row>
-    <row r="291" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="291" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A291" s="2" t="s">
         <v>13</v>
       </c>
@@ -33609,7 +33613,7 @@
         <v>2965</v>
       </c>
     </row>
-    <row r="292" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="292" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A292" s="4" t="s">
         <v>13</v>
       </c>
@@ -33719,7 +33723,7 @@
         <v>4724</v>
       </c>
     </row>
-    <row r="293" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="293" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A293" s="2" t="s">
         <v>13</v>
       </c>
@@ -33829,7 +33833,7 @@
         <v>5750</v>
       </c>
     </row>
-    <row r="294" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="294" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A294" s="4" t="s">
         <v>13</v>
       </c>
@@ -33939,7 +33943,7 @@
         <v>2594</v>
       </c>
     </row>
-    <row r="295" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="295" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A295" s="2" t="s">
         <v>13</v>
       </c>
@@ -34049,7 +34053,7 @@
         <v>3712</v>
       </c>
     </row>
-    <row r="296" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="296" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A296" s="4" t="s">
         <v>9</v>
       </c>
@@ -34159,7 +34163,7 @@
         <v>194967</v>
       </c>
     </row>
-    <row r="297" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="297" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A297" s="2" t="s">
         <v>11</v>
       </c>
@@ -34269,7 +34273,7 @@
         <v>194967</v>
       </c>
     </row>
-    <row r="298" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="298" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A298" s="4" t="s">
         <v>13</v>
       </c>
@@ -34379,7 +34383,7 @@
         <v>16997</v>
       </c>
     </row>
-    <row r="299" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="299" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A299" s="2" t="s">
         <v>13</v>
       </c>
@@ -34489,7 +34493,7 @@
         <v>1396</v>
       </c>
     </row>
-    <row r="300" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="300" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A300" s="4" t="s">
         <v>13</v>
       </c>
@@ -34599,7 +34603,7 @@
         <v>2220</v>
       </c>
     </row>
-    <row r="301" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="301" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A301" s="2" t="s">
         <v>13</v>
       </c>
@@ -34709,7 +34713,7 @@
         <v>2970</v>
       </c>
     </row>
-    <row r="302" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="302" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A302" s="4" t="s">
         <v>13</v>
       </c>
@@ -34819,7 +34823,7 @@
         <v>31497</v>
       </c>
     </row>
-    <row r="303" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="303" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A303" s="2" t="s">
         <v>13</v>
       </c>
@@ -34929,7 +34933,7 @@
         <v>10348</v>
       </c>
     </row>
-    <row r="304" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="304" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A304" s="4" t="s">
         <v>13</v>
       </c>
@@ -35039,7 +35043,7 @@
         <v>11868</v>
       </c>
     </row>
-    <row r="305" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="305" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A305" s="2" t="s">
         <v>13</v>
       </c>
@@ -35149,7 +35153,7 @@
         <v>28690</v>
       </c>
     </row>
-    <row r="306" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="306" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A306" s="4" t="s">
         <v>13</v>
       </c>
@@ -35259,7 +35263,7 @@
         <v>2733</v>
       </c>
     </row>
-    <row r="307" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="307" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A307" s="2" t="s">
         <v>13</v>
       </c>
@@ -35369,7 +35373,7 @@
         <v>17943</v>
       </c>
     </row>
-    <row r="308" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="308" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A308" s="4" t="s">
         <v>13</v>
       </c>
@@ -35479,7 +35483,7 @@
         <v>26037</v>
       </c>
     </row>
-    <row r="309" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="309" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A309" s="2" t="s">
         <v>13</v>
       </c>
@@ -35589,7 +35593,7 @@
         <v>4865</v>
       </c>
     </row>
-    <row r="310" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="310" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A310" s="4" t="s">
         <v>13</v>
       </c>
@@ -35699,7 +35703,7 @@
         <v>15789</v>
       </c>
     </row>
-    <row r="311" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="311" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A311" s="2" t="s">
         <v>13</v>
       </c>
@@ -35809,7 +35813,7 @@
         <v>11502</v>
       </c>
     </row>
-    <row r="312" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="312" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A312" s="4" t="s">
         <v>13</v>
       </c>
@@ -35919,7 +35923,7 @@
         <v>2192</v>
       </c>
     </row>
-    <row r="313" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="313" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A313" s="2" t="s">
         <v>13</v>
       </c>
@@ -36029,7 +36033,7 @@
         <v>7920</v>
       </c>
     </row>
-    <row r="314" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="314" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A314" s="4" t="s">
         <v>7</v>
       </c>
@@ -36139,7 +36143,7 @@
         <v>84084</v>
       </c>
     </row>
-    <row r="315" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="315" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A315" s="2" t="s">
         <v>9</v>
       </c>
@@ -36249,7 +36253,7 @@
         <v>84084</v>
       </c>
     </row>
-    <row r="316" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="316" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A316" s="4" t="s">
         <v>11</v>
       </c>
@@ -36359,7 +36363,7 @@
         <v>1896</v>
       </c>
     </row>
-    <row r="317" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="317" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A317" s="2" t="s">
         <v>13</v>
       </c>
@@ -36469,7 +36473,7 @@
         <v>1896</v>
       </c>
     </row>
-    <row r="318" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="318" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A318" s="4" t="s">
         <v>11</v>
       </c>
@@ -36579,7 +36583,7 @@
         <v>41451</v>
       </c>
     </row>
-    <row r="319" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="319" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A319" s="2" t="s">
         <v>13</v>
       </c>
@@ -36689,7 +36693,7 @@
         <v>4195</v>
       </c>
     </row>
-    <row r="320" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="320" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A320" s="4" t="s">
         <v>13</v>
       </c>
@@ -36799,7 +36803,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="321" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="321" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A321" s="2" t="s">
         <v>13</v>
       </c>
@@ -36909,7 +36913,7 @@
         <v>22789</v>
       </c>
     </row>
-    <row r="322" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="322" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A322" s="4" t="s">
         <v>13</v>
       </c>
@@ -37019,7 +37023,7 @@
         <v>2054</v>
       </c>
     </row>
-    <row r="323" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="323" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A323" s="2" t="s">
         <v>13</v>
       </c>
@@ -37129,7 +37133,7 @@
         <v>7396</v>
       </c>
     </row>
-    <row r="324" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="324" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A324" s="4" t="s">
         <v>13</v>
       </c>
@@ -37239,7 +37243,7 @@
         <v>3229</v>
       </c>
     </row>
-    <row r="325" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="325" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A325" s="2" t="s">
         <v>11</v>
       </c>
@@ -37349,7 +37353,7 @@
         <v>22372</v>
       </c>
     </row>
-    <row r="326" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="326" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A326" s="4" t="s">
         <v>13</v>
       </c>
@@ -37459,7 +37463,7 @@
         <v>14794</v>
       </c>
     </row>
-    <row r="327" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="327" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A327" s="2" t="s">
         <v>13</v>
       </c>
@@ -37569,7 +37573,7 @@
         <v>7578</v>
       </c>
     </row>
-    <row r="328" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="328" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A328" s="4" t="s">
         <v>11</v>
       </c>
@@ -37679,7 +37683,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="329" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="329" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A329" s="2" t="s">
         <v>13</v>
       </c>
@@ -37789,7 +37793,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="330" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="330" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A330" s="4" t="s">
         <v>11</v>
       </c>
@@ -37899,7 +37903,7 @@
         <v>3456</v>
       </c>
     </row>
-    <row r="331" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="331" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A331" s="2" t="s">
         <v>13</v>
       </c>
@@ -38009,7 +38013,7 @@
         <v>1456</v>
       </c>
     </row>
-    <row r="332" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="332" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A332" s="4" t="s">
         <v>13</v>
       </c>
@@ -38119,7 +38123,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="333" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="333" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A333" s="2" t="s">
         <v>11</v>
       </c>
@@ -38229,7 +38233,7 @@
         <v>5711</v>
       </c>
     </row>
-    <row r="334" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="334" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A334" s="4" t="s">
         <v>13</v>
       </c>
@@ -38339,7 +38343,7 @@
         <v>1943</v>
       </c>
     </row>
-    <row r="335" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="335" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A335" s="2" t="s">
         <v>13</v>
       </c>
@@ -38449,7 +38453,7 @@
         <v>2412</v>
       </c>
     </row>
-    <row r="336" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="336" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A336" s="4" t="s">
         <v>13</v>
       </c>
@@ -38559,7 +38563,7 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="337" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="337" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A337" s="2" t="s">
         <v>11</v>
       </c>
@@ -38669,7 +38673,7 @@
         <v>5817</v>
       </c>
     </row>
-    <row r="338" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="338" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A338" s="4" t="s">
         <v>13</v>
       </c>
@@ -38779,7 +38783,7 @@
         <v>5817</v>
       </c>
     </row>
-    <row r="339" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="339" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A339" s="2" t="s">
         <v>11</v>
       </c>
@@ -38889,7 +38893,7 @@
         <v>1361</v>
       </c>
     </row>
-    <row r="340" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="340" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A340" s="4" t="s">
         <v>13</v>
       </c>
@@ -38999,7 +39003,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="341" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="341" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A341" s="2" t="s">
         <v>13</v>
       </c>
@@ -39109,7 +39113,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="342" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="342" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A342" s="4" t="s">
         <v>11</v>
       </c>
@@ -39219,7 +39223,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="343" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="343" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A343" s="2" t="s">
         <v>13</v>
       </c>
@@ -39329,7 +39333,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="344" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="344" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A344" s="4" t="s">
         <v>7</v>
       </c>
@@ -39439,7 +39443,7 @@
         <v>127111</v>
       </c>
     </row>
-    <row r="345" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="345" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A345" s="2" t="s">
         <v>9</v>
       </c>
@@ -39549,7 +39553,7 @@
         <v>127111</v>
       </c>
     </row>
-    <row r="346" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="346" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A346" s="4" t="s">
         <v>11</v>
       </c>
@@ -39659,7 +39663,7 @@
         <v>124319</v>
       </c>
     </row>
-    <row r="347" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="347" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A347" s="2" t="s">
         <v>13</v>
       </c>
@@ -39769,7 +39773,7 @@
         <v>5880</v>
       </c>
     </row>
-    <row r="348" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="348" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A348" s="4" t="s">
         <v>13</v>
       </c>
@@ -39879,7 +39883,7 @@
         <v>14757</v>
       </c>
     </row>
-    <row r="349" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="349" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A349" s="2" t="s">
         <v>13</v>
       </c>
@@ -39989,7 +39993,7 @@
         <v>53880</v>
       </c>
     </row>
-    <row r="350" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="350" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A350" s="4" t="s">
         <v>13</v>
       </c>
@@ -40099,7 +40103,7 @@
         <v>9986</v>
       </c>
     </row>
-    <row r="351" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="351" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A351" s="2" t="s">
         <v>13</v>
       </c>
@@ -40209,7 +40213,7 @@
         <v>4368</v>
       </c>
     </row>
-    <row r="352" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="352" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A352" s="4" t="s">
         <v>13</v>
       </c>
@@ -40319,7 +40323,7 @@
         <v>1677</v>
       </c>
     </row>
-    <row r="353" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="353" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A353" s="2" t="s">
         <v>13</v>
       </c>
@@ -40429,7 +40433,7 @@
         <v>6421</v>
       </c>
     </row>
-    <row r="354" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="354" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A354" s="4" t="s">
         <v>13</v>
       </c>
@@ -40539,7 +40543,7 @@
         <v>21047</v>
       </c>
     </row>
-    <row r="355" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="355" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A355" s="2" t="s">
         <v>13</v>
       </c>
@@ -40649,7 +40653,7 @@
         <v>3625</v>
       </c>
     </row>
-    <row r="356" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="356" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A356" s="4" t="s">
         <v>13</v>
       </c>
@@ -40759,7 +40763,7 @@
         <v>2678</v>
       </c>
     </row>
-    <row r="357" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="357" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A357" s="2" t="s">
         <v>11</v>
       </c>
@@ -40869,7 +40873,7 @@
         <v>2792</v>
       </c>
     </row>
-    <row r="358" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="358" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A358" s="4" t="s">
         <v>13</v>
       </c>
@@ -40979,7 +40983,7 @@
         <v>2792</v>
       </c>
     </row>
-    <row r="359" spans="1:36" ht="14" x14ac:dyDescent="0.15">
+    <row r="359" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A359" s="2" t="s">
         <v>7</v>
       </c>
@@ -41090,6 +41094,14 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:AJ359" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Município"/>
+        <filter val="NUTS III"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:S1"/>

</xml_diff>